<commit_message>
add cascade vals method
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_service.xlsx
+++ b/tests/frameworks/framework_service.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/atomica/tests/frameworks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7B51B896-FEEC-D243-9E92-9C7FDEDB97B2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7D36D4BA-3593-7147-99EC-DAA70C75F485}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compartments" sheetId="2" r:id="rId1"/>
@@ -1323,8 +1323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1497,7 +1497,9 @@
         <v>1</v>
       </c>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
@@ -1743,8 +1745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1879,9 +1881,7 @@
         <v>21</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="H6" s="2">
-        <v>5</v>
-      </c>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">

</xml_diff>

<commit_message>
Update service framework and databook
</commit_message>
<xml_diff>
--- a/tests/frameworks/framework_service.xlsx
+++ b/tests/frameworks/framework_service.xlsx
@@ -1,28 +1,79 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/atomica/tests/frameworks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\frameworks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7D36D4BA-3593-7147-99EC-DAA70C75F485}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83B78897-F4CB-4093-9836-B1A7748B4CA1}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="16095" windowHeight="9660" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Compartments" sheetId="2" r:id="rId1"/>
-    <sheet name="Transitions" sheetId="3" r:id="rId2"/>
-    <sheet name="Characteristics" sheetId="4" r:id="rId3"/>
-    <sheet name="Parameters" sheetId="6" r:id="rId4"/>
+    <sheet name="Databook Pages" sheetId="7" r:id="rId1"/>
+    <sheet name="Compartments" sheetId="2" r:id="rId2"/>
+    <sheet name="Transitions" sheetId="3" r:id="rId3"/>
+    <sheet name="Characteristics" sheetId="4" r:id="rId4"/>
+    <sheet name="Parameters" sheetId="6" r:id="rId5"/>
+    <sheet name="Cascades" sheetId="8" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{A35932FE-AB8C-44E7-9A07-A34A1B2CE922}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column is for the 'code name' of a custom databook sheet.
+Normally, when constructing a databook, data-input sections for
+compartments and characteristics are placed on a single page, while
+parameters are placed on another.
+This section allows custom sheets to be defined, allowing for more
+user-friendly databook organisation.
+Note: A code name is a representative key that developers interface
+with (e.g. in scripts and the codebase).
+It should be in lower case without spaces.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0" xr:uid="{3CA980EF-31C1-40E9-818D-71875E939B5F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>This column is for the title of a custom databook sheet.
+Normally, when constructing a databook, data-input sections for
+compartments and characteristics are placed on a single page, while
+parameters are placed on another.
+This section allows custom sheets to be defined, allowing for more
+user-friendly databook organisation.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -186,7 +237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{5F20F1A1-E77C-42AB-9EFA-D9CD4786F3BF}">
       <text>
         <r>
           <rPr>
@@ -195,9 +246,13 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>This column currently denotes whether a databook should request
-values from the user for the historical size of this compartment.
-A value of '-1' suppresses it from appearing in the databook.</t>
+          <t>This column optionally marks whether a data-input section should
+appear for this compartment in a custom databook sheet, if allowed
+to appear at all according to 'databook order'.
+Each value should be a code name for a desired page defined in
+the 'custom databook pages' worksheet page.
+If a cell is left empty, the enabled data-input section should appear
+in a default databook page dedicated to state variables.</t>
         </r>
       </text>
     </comment>
@@ -232,7 +287,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -355,20 +410,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column defines a 'default_value' attribute for a 'charac' item.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
       <text>
         <r>
           <rPr>
@@ -380,32 +422,6 @@
           <t>This column currently denotes whether a databook should request
 historical values from the user for this characteristic.
 A value of '-1' suppresses it from appearing in the databook.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000009000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This optional column determines what stage of a 'cascade' this
-characteristic corresponds to.
-A cascade is a specific type of compartment network where entities
-flow sequentially from the first compartment to the last.
-A cascade stage is a subset of linked compartments including the
-last in the sequence, where Stage 1 denotes all compartments.
-For instance, with three compartments A, B and C, with transition
-structure A-&gt;B-&gt;C, Stage 1 is the characteristic for (A,B,C),
-Stage 2 is the characteristic for (B,C) and Stage 3 is characteristic
-and compartment (C).
-Note: As exemplified above, one stage should be marked on the
-compartment page, with the rest marked on this page.
-This value is only used for convenience in plotting and the column
-can be safely deleted for non-cascade applications.</t>
         </r>
       </text>
     </comment>
@@ -413,7 +429,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author/>
@@ -567,33 +583,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000004000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column defines a 'default_value' attribute for a 'par' item.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000007000000}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="8"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>This column defines a 'func' attribute for a 'par' item.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000009000000}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000009000000}">
       <text>
         <r>
           <rPr>
@@ -613,7 +603,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="71">
   <si>
     <t>Code Name</t>
   </si>
@@ -633,9 +623,6 @@
     <t>Setup Weight</t>
   </si>
   <si>
-    <t>Databook Order</t>
-  </si>
-  <si>
     <t>Cascade Stage</t>
   </si>
   <si>
@@ -648,15 +635,9 @@
     <t>Denominator</t>
   </si>
   <si>
-    <t>Default Value</t>
-  </si>
-  <si>
     <t>Format</t>
   </si>
   <si>
-    <t>Function</t>
-  </si>
-  <si>
     <t>unaware</t>
   </si>
   <si>
@@ -814,6 +795,27 @@
   </si>
   <si>
     <t>Probability of successful outcome among those receiving services</t>
+  </si>
+  <si>
+    <t>Datasheet Code Name</t>
+  </si>
+  <si>
+    <t>Datasheet Title</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Databook Page</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>Constituents</t>
   </si>
 </sst>
 </file>
@@ -884,7 +886,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -902,6 +904,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1320,26 +1323,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50B013D5-73FB-4398-93EB-8CBA2BAED079}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="A7" sqref="A7:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1359,170 +1398,176 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
       </c>
-      <c r="G2" s="1">
-        <v>-1</v>
-      </c>
+      <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
       </c>
-      <c r="G6" s="2"/>
+      <c r="G6" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="H7" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F8" s="2">
         <v>0</v>
       </c>
-      <c r="G8" s="2">
-        <v>-1</v>
-      </c>
+      <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
   </sheetData>
@@ -1536,7 +1581,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
@@ -1544,12 +1589,12 @@
       <selection activeCell="C2" sqref="C2:H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5"/>
       <c r="B1" s="6" t="str">
         <f>Compartments!$A$2</f>
@@ -1580,14 +1625,14 @@
         <v>dead</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="str">
         <f>Compartments!$A$2</f>
         <v>source</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
@@ -1595,7 +1640,7 @@
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="str">
         <f>Compartments!$A$3</f>
         <v>unaware</v>
@@ -1603,16 +1648,16 @@
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
       <c r="D3" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
       <c r="H3" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="str">
         <f>Compartments!$A$4</f>
         <v>unlinked</v>
@@ -1621,15 +1666,15 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="str">
         <f>Compartments!$A$5</f>
         <v>untx</v>
@@ -1639,14 +1684,14 @@
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="str">
         <f>Compartments!$A$6</f>
         <v>txf</v>
@@ -1657,13 +1702,13 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="str">
         <f>Compartments!$A$7</f>
         <v>txs</v>
@@ -1673,14 +1718,14 @@
       <c r="D7" s="5"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="str">
         <f>Compartments!$A$8</f>
         <v>dead</v>
@@ -1693,7 +1738,7 @@
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
   </sheetData>
@@ -1741,27 +1786,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1772,205 +1815,205 @@
         <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E2" s="4"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F2" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C3" s="4">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E3" s="4"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F3" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C4" s="4">
         <v>1</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E4" s="4"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F4" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E5" s="4"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F5" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C6" s="4">
         <v>1</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="H6" s="2"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F6" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C8" s="4">
         <v>1</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>34</v>
-      </c>
       <c r="B9" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C10" s="4">
         <v>1</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D11" s="4"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
     </row>
@@ -1980,25 +2023,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="63.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2006,139 +2047,127 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D5" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="D6" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="2" t="s">
+      <c r="D7" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="4" t="s">
+      <c r="D8" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2149,4 +2178,71 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B60F2DB1-6AB5-492C-9994-E03A25987B7E}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>